<commit_message>
Added CE and CIRCOMOD project aspects.
</commit_message>
<xml_diff>
--- a/IEDC_Classification_fill/manual_insert/78_RECC_v2.4_CE_Strategies.xlsx
+++ b/IEDC_Classification_fill/manual_insert/78_RECC_v2.4_CE_Strategies.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8018" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8018"/>
   </bookViews>
   <sheets>
     <sheet name="Definition" sheetId="2" r:id="rId1"/>
@@ -731,8 +731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -774,7 +774,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
@@ -938,7 +938,7 @@
         <v>50</v>
       </c>
       <c r="B32" s="2">
-        <v>44877</v>
+        <v>45041</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
@@ -966,7 +966,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T227"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>

</xml_diff>